<commit_message>
completed unit testing according to test plan. 7 test passed
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_investment_account.xlsx
+++ b/tests/A02_pixell_test_plan_investment_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Updated Assignments ISD\assignment_02\given_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralph\OneDrive - Red River College Polytech\Desktop\Intermidiate_Software_Development\Project\Vitug_Ralph_Assignment_1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6AEFC8-F3D7-467B-9A12-00596A3BA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D702C128-C158-479D-9CB0-25C7F7DBE853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="25185" windowHeight="13845" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="10730" yWindow="2070" windowWidth="15180" windowHeight="11910" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -246,6 +246,48 @@
   </si>
   <si>
     <t>date created exactly 10 years ago.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>account_number=2121 client_number=2222 balance=1000.00 date_created=today() management_fee=2.00</t>
+  </si>
+  <si>
+    <t>account_number=2121 client_number=2222 balance=1000.00 date_created=today() management_fee="not_Mark"</t>
+  </si>
+  <si>
+    <t>Object created</t>
+  </si>
+  <si>
+    <t>management_fee=2.00</t>
+  </si>
+  <si>
+    <t>BASE_SERVICE_CHARGE</t>
+  </si>
+  <si>
+    <t>account_number=2121 client_number=2222 balance=1000.00 date_created=(today() - 10 years)</t>
+  </si>
+  <si>
+    <t>account_number=2121 client_number=2222 balance=1000.00 date_created=2024-01-01</t>
+  </si>
+  <si>
+    <t>BASE_SERVICE_CHARGE + 2.00</t>
+  </si>
+  <si>
+    <t>account_number=2121 client_number=2222 balance=1000.00 date_created=2010-01-01</t>
+  </si>
+  <si>
+    <t>BASE_SERVICE_CHARGE and "Management Fee: Waived"</t>
+  </si>
+  <si>
+    <t>Management Fee: Waived</t>
+  </si>
+  <si>
+    <t>Management Fee: $2.00</t>
+  </si>
+  <si>
+    <t>Ralph Vitug</t>
   </si>
 </sst>
 </file>
@@ -552,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -607,6 +649,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,22 +1197,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="27.1796875" customWidth="1"/>
+    <col min="6" max="6" width="28.26953125" customWidth="1"/>
+    <col min="7" max="7" width="49.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="2.15">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1179,14 +1224,16 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1195,10 +1242,10 @@
       </c>
       <c r="D4" s="20"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="11">
         <v>1</v>
       </c>
@@ -1228,11 +1275,17 @@
       <c r="D7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="3">
         <v>2</v>
       </c>
@@ -1242,11 +1295,17 @@
       <c r="D8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="23">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="11">
         <v>3</v>
       </c>
@@ -1256,11 +1315,17 @@
       <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="11">
         <v>4</v>
       </c>
@@ -1270,11 +1335,17 @@
       <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="11">
         <v>5</v>
       </c>
@@ -1284,11 +1355,17 @@
       <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="3">
         <v>6</v>
       </c>
@@ -1298,11 +1375,17 @@
       <c r="D12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1312,11 +1395,17 @@
       <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="11">
         <v>8</v>
       </c>
@@ -1326,7 +1415,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
     </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1336,7 +1425,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="3">
         <v>10</v>
       </c>
@@ -1346,7 +1435,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="11">
         <v>11</v>
       </c>
@@ -1356,7 +1445,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1366,7 +1455,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
         <v>13</v>
       </c>
@@ -1376,7 +1465,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="3">
         <v>14</v>
       </c>
@@ -1386,7 +1475,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1396,7 +1485,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="11">
         <v>16</v>
       </c>
@@ -1406,7 +1495,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="11">
         <v>17</v>
       </c>
@@ -1416,7 +1505,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="3">
         <v>18</v>
       </c>
@@ -1426,7 +1515,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="11">
         <v>19</v>
       </c>
@@ -1436,7 +1525,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="11">
         <v>20</v>
       </c>
@@ -1446,7 +1535,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1456,7 +1545,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="3">
         <v>22</v>
       </c>
@@ -1466,7 +1555,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="11">
         <v>23</v>
       </c>
@@ -1476,7 +1565,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="11">
         <v>24</v>
       </c>
@@ -1486,7 +1575,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="11">
         <v>25</v>
       </c>
@@ -1496,7 +1585,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="3">
         <v>26</v>
       </c>
@@ -1506,7 +1595,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="21" t="s">
         <v>6</v>
       </c>

</xml_diff>